<commit_message>
build basic UI frame
</commit_message>
<xml_diff>
--- a/docs/01-Desgin/01-FeatureList.xlsx
+++ b/docs/01-Desgin/01-FeatureList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>功能点列表</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -32,10 +32,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>工作量</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>功能点</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -237,6 +233,22 @@
   </si>
   <si>
     <t>播放功能</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>定制听</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>下载听</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>我</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>工作量（人/天）</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -514,25 +526,13 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -544,17 +544,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -565,9 +556,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -585,6 +573,39 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -892,11 +913,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D1:O62"/>
+  <dimension ref="D1:O65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G39" sqref="G39"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -905,509 +926,514 @@
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.75" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43" customWidth="1"/>
+    <col min="9" max="9" width="22.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:15" ht="45" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
     </row>
     <row r="2" spans="4:15" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="4:15" ht="19.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="31" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="4:15" ht="19.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="20"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="4:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D4" s="31"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" spans="4:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D5" s="31"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="4:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="31"/>
+      <c r="E6" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="8"/>
+    </row>
+    <row r="7" spans="4:15" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="31"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="8"/>
+    </row>
+    <row r="8" spans="4:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="31"/>
+      <c r="E8" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="4:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D9" s="31"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="4:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D10" s="31"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="4:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D11" s="31"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="7"/>
+      <c r="I11" s="8"/>
+    </row>
+    <row r="12" spans="4:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D12" s="31"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="I12" s="8"/>
+    </row>
+    <row r="13" spans="4:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D13" s="31"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="7"/>
+      <c r="I13" s="8"/>
+    </row>
+    <row r="14" spans="4:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D14" s="31"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="8"/>
+    </row>
+    <row r="15" spans="4:15" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D15" s="31"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" s="9"/>
+      <c r="I15" s="10"/>
+      <c r="O15"/>
+    </row>
+    <row r="16" spans="4:15" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D16" s="31"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="9"/>
+      <c r="I16" s="10"/>
+      <c r="O16"/>
+    </row>
+    <row r="17" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D17" s="31"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="7"/>
+      <c r="I17" s="8"/>
+    </row>
+    <row r="18" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D18" s="31"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="7"/>
+      <c r="I18" s="8"/>
+    </row>
+    <row r="19" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D19" s="31"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="7"/>
+      <c r="I19" s="8"/>
+    </row>
+    <row r="20" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D20" s="31"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="I20" s="8"/>
+    </row>
+    <row r="21" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D21" s="31"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" s="7"/>
+      <c r="I21" s="8"/>
+    </row>
+    <row r="22" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D22" s="31"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22" s="8"/>
+    </row>
+    <row r="23" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D23" s="31"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23" s="7"/>
+      <c r="I23" s="8"/>
+    </row>
+    <row r="24" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D24" s="31"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H24" s="7"/>
+      <c r="I24" s="8"/>
+    </row>
+    <row r="25" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D25" s="31"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H25" s="7"/>
+      <c r="I25" s="8"/>
+    </row>
+    <row r="26" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D26" s="31"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H26" s="7"/>
+      <c r="I26" s="8"/>
+    </row>
+    <row r="27" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D27" s="31"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H27" s="7"/>
+      <c r="I27" s="8"/>
+    </row>
+    <row r="28" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D28" s="31"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H28" s="7"/>
+      <c r="I28" s="8"/>
+    </row>
+    <row r="29" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D29" s="31"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H29" s="7"/>
+      <c r="I29" s="8"/>
+    </row>
+    <row r="30" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D30" s="31"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H30" s="7"/>
+      <c r="I30" s="8"/>
+    </row>
+    <row r="31" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D31" s="31"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H31" s="7"/>
+      <c r="I31" s="8"/>
+    </row>
+    <row r="32" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D32" s="31"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H32" s="7"/>
+      <c r="I32" s="8"/>
+    </row>
+    <row r="33" spans="4:13" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D33" s="31"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H33" s="7"/>
+      <c r="I33" s="8"/>
+    </row>
+    <row r="34" spans="4:13" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D34" s="31"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H34" s="7"/>
+      <c r="I34" s="8"/>
+    </row>
+    <row r="35" spans="4:13" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D35" s="31"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H35" s="7"/>
+      <c r="I35" s="8"/>
+    </row>
+    <row r="36" spans="4:13" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D36" s="31"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H36" s="7"/>
+      <c r="I36" s="8"/>
+    </row>
+    <row r="37" spans="4:13" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D37" s="31"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H37" s="7"/>
+      <c r="I37" s="8"/>
+    </row>
+    <row r="38" spans="4:13" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D38" s="31"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H38" s="7"/>
+      <c r="I38" s="8"/>
+    </row>
+    <row r="39" spans="4:13" ht="57.75" x14ac:dyDescent="0.25">
+      <c r="D39" s="24"/>
+      <c r="E39" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F39" s="18"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="8"/>
+    </row>
+    <row r="40" spans="4:13" ht="57.75" x14ac:dyDescent="0.25">
+      <c r="D40" s="24"/>
+      <c r="E40" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F40" s="18"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="8"/>
+    </row>
+    <row r="41" spans="4:13" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="D41" s="24"/>
+      <c r="E41" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F41" s="18"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="8"/>
+    </row>
+    <row r="42" spans="4:13" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D42" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="9"/>
-    </row>
-    <row r="4" spans="4:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D4" s="32"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="12"/>
-    </row>
-    <row r="5" spans="4:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D5" s="32"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="12"/>
-    </row>
-    <row r="6" spans="4:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="32"/>
-      <c r="E6" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="12"/>
-    </row>
-    <row r="7" spans="4:15" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="32"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="12"/>
-    </row>
-    <row r="8" spans="4:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="32"/>
-      <c r="E8" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="12"/>
-    </row>
-    <row r="9" spans="4:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D9" s="32"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="11"/>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="4:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D10" s="32"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="12"/>
-    </row>
-    <row r="11" spans="4:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D11" s="32"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="12"/>
-    </row>
-    <row r="12" spans="4:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D12" s="32"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="12"/>
-    </row>
-    <row r="13" spans="4:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D13" s="32"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" s="11"/>
-      <c r="I13" s="12"/>
-    </row>
-    <row r="14" spans="4:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D14" s="32"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="12"/>
-    </row>
-    <row r="15" spans="4:15" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D15" s="32"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H15" s="13"/>
-      <c r="I15" s="14"/>
-      <c r="O15"/>
-    </row>
-    <row r="16" spans="4:15" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D16" s="32"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="H16" s="13"/>
-      <c r="I16" s="14"/>
-      <c r="O16"/>
-    </row>
-    <row r="17" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D17" s="32"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="H17" s="11"/>
-      <c r="I17" s="12"/>
-    </row>
-    <row r="18" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D18" s="32"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="H18" s="11"/>
-      <c r="I18" s="12"/>
-    </row>
-    <row r="19" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D19" s="32"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H19" s="11"/>
-      <c r="I19" s="12"/>
-    </row>
-    <row r="20" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D20" s="32"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="H20" s="11"/>
-      <c r="I20" s="12"/>
-    </row>
-    <row r="21" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D21" s="32"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H21" s="11"/>
-      <c r="I21" s="12"/>
-    </row>
-    <row r="22" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D22" s="32"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="H22" s="11"/>
-      <c r="I22" s="12"/>
-    </row>
-    <row r="23" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D23" s="32"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H23" s="11"/>
-      <c r="I23" s="12"/>
-    </row>
-    <row r="24" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D24" s="32"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="H24" s="11"/>
-      <c r="I24" s="12"/>
-    </row>
-    <row r="25" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D25" s="32"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H25" s="11"/>
-      <c r="I25" s="12"/>
-    </row>
-    <row r="26" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D26" s="32"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="H26" s="11"/>
-      <c r="I26" s="12"/>
-    </row>
-    <row r="27" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D27" s="32"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="H27" s="11"/>
-      <c r="I27" s="12"/>
-    </row>
-    <row r="28" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D28" s="32"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="H28" s="11"/>
-      <c r="I28" s="12"/>
-    </row>
-    <row r="29" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D29" s="32"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H29" s="11"/>
-      <c r="I29" s="12"/>
-    </row>
-    <row r="30" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D30" s="32"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="H30" s="11"/>
-      <c r="I30" s="12"/>
-    </row>
-    <row r="31" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D31" s="32"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="H31" s="11"/>
-      <c r="I31" s="12"/>
-    </row>
-    <row r="32" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D32" s="32"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="H32" s="11"/>
-      <c r="I32" s="12"/>
-    </row>
-    <row r="33" spans="4:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D33" s="32"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H33" s="11"/>
-      <c r="I33" s="12"/>
-    </row>
-    <row r="34" spans="4:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D34" s="32"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="H34" s="11"/>
-      <c r="I34" s="12"/>
-    </row>
-    <row r="35" spans="4:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D35" s="32"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="H35" s="11"/>
-      <c r="I35" s="12"/>
-    </row>
-    <row r="36" spans="4:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D36" s="32"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="H36" s="11"/>
-      <c r="I36" s="12"/>
-    </row>
-    <row r="37" spans="4:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D37" s="32"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="H37" s="11"/>
-      <c r="I37" s="12"/>
-    </row>
-    <row r="38" spans="4:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D38" s="32"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="G38" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="H38" s="11"/>
-      <c r="I38" s="12"/>
-    </row>
-    <row r="39" spans="4:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D39" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="19"/>
-    </row>
-    <row r="40" spans="4:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D40" s="20"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="12"/>
-    </row>
-    <row r="41" spans="4:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D41" s="20"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="12"/>
-    </row>
-    <row r="42" spans="4:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D42" s="20"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="12"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="14"/>
     </row>
     <row r="43" spans="4:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D43" s="20"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="12"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="8"/>
     </row>
     <row r="44" spans="4:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D44" s="20"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="12"/>
-      <c r="M44" s="2"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="8"/>
     </row>
     <row r="45" spans="4:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D45" s="20"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="12"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="8"/>
     </row>
     <row r="46" spans="4:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D46" s="21"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="15"/>
-      <c r="H46" s="15"/>
-      <c r="I46" s="16"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="8"/>
     </row>
     <row r="47" spans="4:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D47" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="18"/>
-      <c r="I47" s="19"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="8"/>
+      <c r="M47" s="2"/>
     </row>
     <row r="48" spans="4:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D48" s="20"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="12"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="8"/>
     </row>
     <row r="49" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D49" s="20"/>
+      <c r="D49" s="27"/>
       <c r="E49" s="11"/>
       <c r="F49" s="11"/>
       <c r="G49" s="11"/>
@@ -1415,63 +1441,65 @@
       <c r="I49" s="12"/>
     </row>
     <row r="50" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D50" s="20"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="12"/>
+      <c r="D50" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="14"/>
     </row>
     <row r="51" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D51" s="20"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="12"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
+      <c r="I51" s="8"/>
     </row>
     <row r="52" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D52" s="20"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="12"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+      <c r="I52" s="8"/>
     </row>
     <row r="53" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="20"/>
-      <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11"/>
-      <c r="I53" s="12"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
+      <c r="I53" s="8"/>
     </row>
     <row r="54" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="21"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="15"/>
-      <c r="H54" s="15"/>
-      <c r="I54" s="16"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+      <c r="I54" s="8"/>
     </row>
     <row r="55" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D55" s="17"/>
-      <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="11"/>
-      <c r="I55" s="12"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+      <c r="I55" s="8"/>
     </row>
     <row r="56" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D56" s="20"/>
-      <c r="E56" s="11"/>
-      <c r="F56" s="11"/>
-      <c r="G56" s="11"/>
-      <c r="H56" s="11"/>
-      <c r="I56" s="12"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
+      <c r="I56" s="8"/>
     </row>
     <row r="57" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D57" s="20"/>
+      <c r="D57" s="27"/>
       <c r="E57" s="11"/>
       <c r="F57" s="11"/>
       <c r="G57" s="11"/>
@@ -1479,50 +1507,75 @@
       <c r="I57" s="12"/>
     </row>
     <row r="58" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D58" s="20"/>
-      <c r="E58" s="11"/>
-      <c r="F58" s="11"/>
-      <c r="G58" s="11"/>
-      <c r="H58" s="11"/>
-      <c r="I58" s="12"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7"/>
+      <c r="I58" s="8"/>
     </row>
     <row r="59" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D59" s="20"/>
-      <c r="E59" s="11"/>
-      <c r="F59" s="11"/>
-      <c r="G59" s="11"/>
-      <c r="H59" s="11"/>
-      <c r="I59" s="12"/>
+      <c r="D59" s="26"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="7"/>
+      <c r="I59" s="8"/>
     </row>
     <row r="60" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D60" s="20"/>
-      <c r="E60" s="11"/>
-      <c r="F60" s="11"/>
-      <c r="G60" s="11"/>
-      <c r="H60" s="11"/>
-      <c r="I60" s="12"/>
+      <c r="D60" s="26"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
+      <c r="H60" s="7"/>
+      <c r="I60" s="8"/>
     </row>
     <row r="61" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D61" s="20"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="11"/>
-      <c r="I61" s="12"/>
+      <c r="D61" s="26"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
+      <c r="H61" s="7"/>
+      <c r="I61" s="8"/>
     </row>
     <row r="62" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D62" s="21"/>
-      <c r="E62" s="15"/>
-      <c r="F62" s="15"/>
-      <c r="G62" s="15"/>
-      <c r="H62" s="15"/>
-      <c r="I62" s="16"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="7"/>
+      <c r="I62" s="8"/>
+    </row>
+    <row r="63" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D63" s="26"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="7"/>
+      <c r="H63" s="7"/>
+      <c r="I63" s="8"/>
+    </row>
+    <row r="64" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D64" s="26"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
+      <c r="I64" s="8"/>
+    </row>
+    <row r="65" spans="4:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D65" s="27"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="11"/>
+      <c r="I65" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D55:D62"/>
-    <mergeCell ref="D47:D54"/>
-    <mergeCell ref="D39:D46"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="D58:D65"/>
+    <mergeCell ref="D50:D57"/>
+    <mergeCell ref="D42:D49"/>
     <mergeCell ref="F18:F22"/>
     <mergeCell ref="F23:F24"/>
     <mergeCell ref="E8:E38"/>
@@ -1533,7 +1586,6 @@
     <mergeCell ref="F8:F13"/>
     <mergeCell ref="E3:E5"/>
     <mergeCell ref="E6:E7"/>
-    <mergeCell ref="D1:I1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>